<commit_message>
Iteration 2 major revise
</commit_message>
<xml_diff>
--- a/Iteration 1/6. ERROR LOGS/defect_log.xlsx
+++ b/Iteration 1/6. ERROR LOGS/defect_log.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\ICT Courses material\BCPR280 Software Engineering 2\BCPR280_Software_Engineering_2_Assignment1\Iteration 1\6. ERROR LOGS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCPR280_Software_Engineering_2_Assignment1\Iteration 1\6. ERROR LOGS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8157A6-4C63-4C0B-AD9D-ED4913E87131}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="432" windowWidth="19872" windowHeight="7716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="435" windowWidth="19875" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="reason" localSheetId="0">Sheet1!$A$85</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="156">
   <si>
     <t>PSP Defect Recording Log</t>
   </si>
@@ -619,9 +621,6 @@
     <t>Michael, Luofeng</t>
   </si>
   <si>
-    <t>did not use Jasmine matcher to copare the value, so the message appeared: "has no expectations"</t>
-  </si>
-  <si>
     <t>MA</t>
   </si>
   <si>
@@ -631,14 +630,608 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Did not assign a predetermined values to the test case</t>
+    <t>Did not assign predetermined values to the test case</t>
+  </si>
+  <si>
+    <t>design</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Did not put } for an anonymous function, should be () =&gt; {}</t>
+  </si>
+  <si>
+    <t>Wrong object name, "gueser1" shoud be "guesser1"</t>
+  </si>
+  <si>
+    <t>Redraw class diagram. The structure of Vue object is different from plain JS object</t>
+  </si>
+  <si>
+    <t>did not use toEqual () to copare the value, so the message appeared: "has no expectations"</t>
+  </si>
+  <si>
+    <t>did not use toBeTruthy () to copare the value, so the message appeared: "has no expectations"</t>
+  </si>
+  <si>
+    <t>Did not call compareNumber(), so the counter didn't add up</t>
+  </si>
+  <si>
+    <t>Did not enclose it(``, () =&gt; {}) properly</t>
+  </si>
+  <si>
+    <t>Defect Types</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This classification describes the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>structure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> of the defect: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>IC:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Interface Capability.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The design of an interface is wrong, so that the interface does not provide the functionality that it must provide. </t>
+  </si>
+  <si>
+    <r>
+      <t>IS:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Interface Specification.</t>
+    </r>
+  </si>
+  <si>
+    <t>The specification of an interface is wrong, so that the parameters involved cannot transfer all of the information required for providing the intended functionality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a less fundamental variant of IC: Only parameters need be added. </t>
+  </si>
+  <si>
+    <r>
+      <t>ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Interface Description.</t>
+    </r>
+  </si>
+  <si>
+    <t>The non-formal part of the description of an interface is incomplete, wrong, or misleading. This is typically diagnosed after an IU.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note that the description of a variable or class attribute or data structure invariant is also an (internal) interface. </t>
+  </si>
+  <si>
+    <r>
+      <t>II:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Interface Implementation.</t>
+    </r>
+  </si>
+  <si>
+    <t>Something that I cannot influence does not work as it should.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This defect should never be used when I am the source of the defect. (In principle, this is a special case of ID.) </t>
+  </si>
+  <si>
+    <r>
+      <t>IU:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Interface Use.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">An interface was used wrongly, i.e., in such a way as to violate the interface specification. </t>
+  </si>
+  <si>
+    <r>
+      <t>IV:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Data Invariant.</t>
+    </r>
+  </si>
+  <si>
+    <t>A special case of IU. The interface violation is: not maintaining the invariant of some variable or data structure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Violating the meaning of a simple variable is a special case of this. </t>
+  </si>
+  <si>
+    <r>
+      <t>MD:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Missing Design (of required functionality).</t>
+    </r>
+  </si>
+  <si>
+    <t>A certain requirement is covered nowhere in the design.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is stronger than IC, where the coverage is present, but incomplete. </t>
+  </si>
+  <si>
+    <r>
+      <t>MI:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Missing Implementation (of planned functionality).</t>
+    </r>
+  </si>
+  <si>
+    <t>A certain part of a design was not implemented.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the part is small, MC, MA or WA may be more appropriate. </t>
+  </si>
+  <si>
+    <r>
+      <t>ME:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Missed Errorhandling.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">An error case was not handled in the program (or not handled properly). </t>
+  </si>
+  <si>
+    <r>
+      <t>MA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Missing Assignment.</t>
+    </r>
+  </si>
+  <si>
+    <t>A single variable was not initialized or updated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only one statement needs to be added. </t>
+  </si>
+  <si>
+    <r>
+      <t>MC:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Missing Call.</t>
+    </r>
+  </si>
+  <si>
+    <t>A single method call is missing.</t>
+  </si>
+  <si>
+    <r>
+      <t>WA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Wrong Algorithm.</t>
+    </r>
+  </si>
+  <si>
+    <t>The entire logic in a method is wrong and cannot provide the desired functionality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More than one statement needs to be added or changed. </t>
+  </si>
+  <si>
+    <r>
+      <t>WE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Wrong Expression.</t>
+    </r>
+  </si>
+  <si>
+    <t>An expression (in an assignment or method call) computes the wrong value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only one expression needs to be changed. </t>
+  </si>
+  <si>
+    <r>
+      <t>WC:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Wrong Condition.</t>
+    </r>
+  </si>
+  <si>
+    <t>Special case of WE. A boolean expression was wrong.</t>
+  </si>
+  <si>
+    <r>
+      <t>WN:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Wrong Name.</t>
+    </r>
+  </si>
+  <si>
+    <t>Special case of WE. Objects or their names were confused. The wrong method, attribute, or variable was used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only one name needs to be changed. </t>
+  </si>
+  <si>
+    <r>
+      <t>WT:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Wrong Type.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Two `similar' types were confused. </t>
+  </si>
+  <si>
+    <t>IC, IS, ID, MD are typically related to design.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IU, IV, MI, MA, WE, WC, WN are typically related to implementation. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">After some defect data have been collected one may adapt the above classification to one's own needs. Such changes should be upwards compatible so as not to render old data useless. This means that the only changes are typically </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>clarification</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> of the definition of a defect type and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>extension</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> of the scheme to include additional defect types. Old defect types may be marked obsolete but should not be removed from the standard. Still, as a rule, changes to the defect classification should be made only rarely. </t>
+    </r>
+  </si>
+  <si>
+    <t>Defect Reasons</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This classification describes </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>why the defect was introduced</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>om:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Omission.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">I forgot something that I knew I had to do. </t>
+  </si>
+  <si>
+    <r>
+      <t>ig:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Ignorance.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">I forgot something, because I did not know I had to do it. </t>
+  </si>
+  <si>
+    <r>
+      <t>cm:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Commission.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">I did something wrong, although I knew in principle how to do it right. </t>
+  </si>
+  <si>
+    <r>
+      <t>ty:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Typo.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">I did something trivial wrong, although I knew exactly how to do it right. </t>
+  </si>
+  <si>
+    <r>
+      <t>kn:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Knowledge.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">I did something wrong, because I lacked the general knowledge (i.e., the education) how to do it right. </t>
+  </si>
+  <si>
+    <r>
+      <t>in:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Information.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">I did something wrong, because I lacked the specific knowledge how to do it right or had received misleading information about how to do it. This refers to a problem with communication. </t>
+  </si>
+  <si>
+    <r>
+      <t>ex:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> External.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">I did nothing wrong. The problem was somewhere else and the defect was introduced by some other person. </t>
+  </si>
+  <si>
+    <t>comparsion should be (0 &lt;= theNumber &amp;&amp; theNumber &lt; 100) instead of (0 &lt; theNumber &amp;&amp; theNumber &lt; 100)</t>
+  </si>
+  <si>
+    <t>2min</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>WC</t>
+  </si>
+  <si>
+    <t>MI-ty</t>
+  </si>
+  <si>
+    <t>Forget to update attribute "counter"</t>
+  </si>
+  <si>
+    <t>MD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -702,6 +1295,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF365F91"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -894,7 +1520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -959,6 +1585,30 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1054,23 +1704,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1106,23 +1739,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1298,28 +1914,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" customWidth="1"/>
-    <col min="8" max="8" width="80.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="80.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1327,7 +1944,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1335,7 +1952,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1343,7 +1960,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1369,252 +1986,736 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>43316</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>155</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>67</v>
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
+        <v>78</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>43316</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
         <v>64</v>
       </c>
       <c r="E8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>43316</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
         <v>64</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>43316</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" t="s">
         <v>74</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H10" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="H8" s="6" t="s">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <v>43316</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <v>43316</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>43316</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>7</v>
-      </c>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13">
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>43316</v>
+      </c>
+      <c r="B14">
         <v>8</v>
       </c>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B14">
+      <c r="C14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>43316</v>
+      </c>
+      <c r="B15">
         <v>9</v>
       </c>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B15">
+      <c r="C15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>43316</v>
+      </c>
+      <c r="B16">
         <v>10</v>
       </c>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>86</v>
+      </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>87</v>
+      </c>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>88</v>
+      </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>89</v>
+      </c>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="30"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>90</v>
+      </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>91</v>
+      </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>92</v>
+      </c>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>94</v>
+      </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
+        <v>95</v>
+      </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
+        <v>96</v>
+      </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>97</v>
+      </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>98</v>
+      </c>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="30"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
+        <v>99</v>
+      </c>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="30"/>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
+        <v>102</v>
+      </c>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="32" t="s">
+        <v>103</v>
+      </c>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="30"/>
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
+        <v>104</v>
+      </c>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
+        <v>105</v>
+      </c>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
+        <v>106</v>
+      </c>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="30"/>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="31" t="s">
+        <v>107</v>
+      </c>
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
+        <v>108</v>
+      </c>
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
+        <v>109</v>
+      </c>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="30"/>
       <c r="H51" s="6"/>
     </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="31" t="s">
+        <v>110</v>
+      </c>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
+        <v>111</v>
+      </c>
       <c r="H53" s="6"/>
     </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="30"/>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="31" t="s">
+        <v>112</v>
+      </c>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="32" t="s">
+        <v>113</v>
+      </c>
       <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="30"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="30"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="30"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="30"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="30"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="30"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A87" s="26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="30"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="30"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="30"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="30"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="30"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="31" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="30"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="30"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="32" t="s">
+        <v>148</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1" xr:uid="{4CFD0A15-7F9C-4840-A8B0-9804F97EB694}"/>
+    <hyperlink ref="G8" r:id="rId1"/>
+    <hyperlink ref="G9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="125" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="91" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="91" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78" customWidth="1"/>
-    <col min="3" max="3" width="54.44140625" customWidth="1"/>
+    <col min="3" max="3" width="54.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>13</v>
       </c>
@@ -1622,13 +2723,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
       <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>16</v>
       </c>
@@ -1636,13 +2737,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
       <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>19</v>
       </c>
@@ -1650,19 +2751,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21"/>
       <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>23</v>
       </c>
@@ -1670,13 +2771,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
       <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>4</v>
       </c>
@@ -1684,7 +2785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>27</v>
       </c>
@@ -1692,13 +2793,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21"/>
       <c r="B13" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>5</v>
       </c>
@@ -1706,13 +2807,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
       <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>6</v>
       </c>
@@ -1720,13 +2821,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21"/>
       <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>7</v>
       </c>
@@ -1734,7 +2835,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>8</v>
       </c>
@@ -1742,13 +2843,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21"/>
       <c r="B20" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>37</v>
       </c>
@@ -1756,13 +2857,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21"/>
       <c r="B22" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>10</v>
       </c>
@@ -1770,18 +2871,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>41</v>
       </c>
@@ -1792,7 +2893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17">
         <v>10</v>
       </c>
@@ -1803,7 +2904,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17">
         <v>20</v>
       </c>
@@ -1814,7 +2915,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17">
         <v>30</v>
       </c>
@@ -1825,7 +2926,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
         <v>40</v>
       </c>
@@ -1836,7 +2937,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17">
         <v>50</v>
       </c>
@@ -1847,7 +2948,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17">
         <v>60</v>
       </c>
@@ -1858,7 +2959,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17">
         <v>70</v>
       </c>
@@ -1869,7 +2970,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17">
         <v>80</v>
       </c>
@@ -1880,7 +2981,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17">
         <v>90</v>
       </c>
@@ -1891,7 +2992,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17">
         <v>100</v>
       </c>
@@ -1902,7 +3003,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
     </row>
   </sheetData>

</xml_diff>